<commit_message>
feat(Director#addProjectPaper): paper를 받는 기능 및 테스트 구현
</commit_message>
<xml_diff>
--- a/docs/doctor.xlsx
+++ b/docs/doctor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\is2js\IdeaProjects\object\doctor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE740E4F-5631-4B36-9B74-EE0081D47102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A85FEBF-9F6A-418E-B265-B4FB6EA1B615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5232" yWindow="2448" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{30BBED63-F7C0-40C5-866E-E705D16EC134}"/>
   </bookViews>
@@ -544,10 +544,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. director는 [외부]에서 기획서를 [받기기능]으로 받아서 저장하므로 안다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>director.addPaper( paper )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -676,6 +672,10 @@
   </si>
   <si>
     <t>5. 디렉터는 내부생성 하위도메인 Programmer +  외부에서 받아오는 ProjectPaper를 가지고 [외부에 getter최종프로그램반환 제공기능]하며</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. director는 [외부]에서 기획서를 [void setter 여러 개add 받기기능]으로 받아서 저장하므로 안다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -13694,8 +13694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B10D1B8-D54B-4833-A6DD-E681E2374463}">
   <dimension ref="D3:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M74" sqref="M74"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -13776,7 +13776,7 @@
     </row>
     <row r="20" spans="8:12">
       <c r="J20" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="8:12" ht="18" thickBot="1">
@@ -13790,7 +13790,7 @@
       </c>
       <c r="I22" s="6"/>
       <c r="L22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="8:12" ht="18" thickBot="1"/>
@@ -13811,13 +13811,13 @@
     <row r="33" spans="4:18" ht="18" thickBot="1">
       <c r="E33" s="7"/>
       <c r="F33" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K33" s="6"/>
       <c r="L33" s="7"/>
@@ -13832,23 +13832,23 @@
     </row>
     <row r="35" spans="4:18">
       <c r="E35" t="s">
+        <v>108</v>
+      </c>
+      <c r="L35" t="s">
         <v>109</v>
-      </c>
-      <c r="L35" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="36" spans="4:18">
       <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="L36" t="s">
         <v>111</v>
-      </c>
-      <c r="L36" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="37" spans="4:18" ht="18" thickBot="1">
       <c r="K37" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="4:18" ht="18" thickBot="1">
@@ -13857,12 +13857,12 @@
       </c>
       <c r="I38" s="6"/>
       <c r="K38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="4:18">
       <c r="N39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="4:18" ht="18" thickBot="1"/>
@@ -13872,13 +13872,13 @@
       </c>
       <c r="I41" s="6"/>
       <c r="N41" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O41" s="6"/>
     </row>
     <row r="42" spans="4:18" ht="18" thickBot="1">
       <c r="R42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="4:18" ht="18" thickBot="1">
@@ -13889,15 +13889,15 @@
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K43" s="6"/>
       <c r="M43" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N43" s="6"/>
       <c r="P43" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q43" s="6"/>
     </row>
@@ -13910,12 +13910,12 @@
     </row>
     <row r="52" spans="6:22">
       <c r="N52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="6:22" ht="18" thickBot="1">
       <c r="R53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="6:22" ht="18" thickBot="1">
@@ -13924,11 +13924,11 @@
       </c>
       <c r="I54" s="6"/>
       <c r="N54" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O54" s="6"/>
       <c r="R54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="6:22" ht="18" thickBot="1"/>
@@ -13940,21 +13940,21 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K56" s="6"/>
       <c r="M56" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N56" s="6"/>
       <c r="P56" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q56" s="6"/>
     </row>
     <row r="63" spans="6:22" ht="18" thickBot="1">
       <c r="V63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="6:22" ht="18" thickBot="1">
@@ -13963,17 +13963,17 @@
       </c>
       <c r="I64" s="6"/>
       <c r="M64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="6:17">
       <c r="O65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="6:17" ht="18" thickBot="1">
       <c r="Q66" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="6:17" ht="18" thickBot="1">
@@ -13982,7 +13982,7 @@
       </c>
       <c r="I67" s="6"/>
       <c r="N67" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O67" s="6"/>
     </row>
@@ -13995,15 +13995,15 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K69" s="6"/>
       <c r="M69" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N69" s="6"/>
       <c r="P69" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q69" s="6"/>
     </row>

</xml_diff>